<commit_message>
Refreshed list of finished exsersises
</commit_message>
<xml_diff>
--- a/5kurs/Perechen_otchetnosti.xlsx
+++ b/5kurs/Perechen_otchetnosti.xlsx
@@ -521,7 +521,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,7 +557,7 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="5" t="s">

</xml_diff>

<commit_message>
Added referats and article
</commit_message>
<xml_diff>
--- a/5kurs/Perechen_otchetnosti.xlsx
+++ b/5kurs/Perechen_otchetnosti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11430"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,7 +665,7 @@
       <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -682,7 +682,7 @@
       <c r="D9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
       <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Checked Refereat for UPRITS
</commit_message>
<xml_diff>
--- a/5kurs/Perechen_otchetnosti.xlsx
+++ b/5kurs/Perechen_otchetnosti.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -614,13 +614,13 @@
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished presentation for PPR
</commit_message>
<xml_diff>
--- a/5kurs/Perechen_otchetnosti.xlsx
+++ b/5kurs/Perechen_otchetnosti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11430"/>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -600,7 +600,7 @@
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -617,7 +617,7 @@
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -634,7 +634,7 @@
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -654,7 +654,7 @@
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="4" t="s">

</xml_diff>

<commit_message>
Added Predein's referat for EB
</commit_message>
<xml_diff>
--- a/5kurs/Perechen_otchetnosti.xlsx
+++ b/5kurs/Perechen_otchetnosti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11430"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,7 +668,7 @@
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="5" t="s">

</xml_diff>

<commit_message>
Finished presentation for article
</commit_message>
<xml_diff>
--- a/5kurs/Perechen_otchetnosti.xlsx
+++ b/5kurs/Perechen_otchetnosti.xlsx
@@ -220,16 +220,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -527,7 +526,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,13 +562,13 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -583,10 +582,10 @@
       <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -597,13 +596,13 @@
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -614,13 +613,13 @@
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -631,13 +630,13 @@
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -648,13 +647,13 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -665,13 +664,13 @@
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -682,13 +681,13 @@
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -699,23 +698,23 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>